<commit_message>
tunnel plots, sigmoid, tables
</commit_message>
<xml_diff>
--- a/error-compare.xlsx
+++ b/error-compare.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sterg\Documents\GitHub\infer\code\interp\code\interp5DOF-paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE127553-925E-422F-91FD-E740D5C5B662}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC673420-D59A-4C69-A345-41DCA8579356}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3FFA48DE-A732-4E48-AC34-6AA140314E0A}"/>
   </bookViews>
@@ -87,9 +87,6 @@
     <t>\gls{lobpcg} \cite{shenDeterminingGrainBoundary2019}</t>
   </si>
   <si>
-    <t>\gls{ann} \cite{echeverrirestrepoUsingArtificialNeural2014}</t>
-  </si>
-  <si>
     <t>\gls{lkr} \cite{chesserLearningGrainBoundary2020}</t>
   </si>
   <si>
@@ -157,14 +154,18 @@
   </si>
   <si>
     <t>\NA</t>
+  </si>
+  <si>
+    <t>\gls{ann} \cite{restrepoUsingArtificialNeural2014}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.0%"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -236,22 +237,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="7">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -383,64 +443,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -452,10 +454,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -484,23 +482,23 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{50286348-A0AD-4367-867A-FF703B492F79}" name="Table2" displayName="Table2" ref="I13:N21" totalsRowShown="0" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{50286348-A0AD-4367-867A-FF703B492F79}" name="Table2" displayName="Table2" ref="I13:N21" totalsRowShown="0" dataDxfId="6">
   <autoFilter ref="I13:N21" xr:uid="{62E6D853-2620-453D-94A0-2A9CC9A67D6A}"/>
   <tableColumns count="6">
-    <tableColumn id="6" xr3:uid="{A9D0C93B-0EA4-4493-91CC-FEFD3AE97CC7}" name="Column1" dataDxfId="3"/>
-    <tableColumn id="1" xr3:uid="{3314CF19-98B3-4633-8C5D-306394963DCF}" name="Column2" dataDxfId="2">
+    <tableColumn id="6" xr3:uid="{A9D0C93B-0EA4-4493-91CC-FEFD3AE97CC7}" name="Column1" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{3314CF19-98B3-4633-8C5D-306394963DCF}" name="Column2" dataDxfId="4">
       <calculatedColumnFormula>_xlfn.TEXTJOIN(,TRUE,A14,C14,H14)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{62BC181E-E540-457E-8A83-80B02351069D}" name="Column3" dataDxfId="0">
+    <tableColumn id="2" xr3:uid="{62BC181E-E540-457E-8A83-80B02351069D}" name="Column3" dataDxfId="3">
       <calculatedColumnFormula>_xlfn.TEXTJOIN(,TRUE,$A14,D14,$H14)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{288D3A6C-7636-4CB2-9C87-1538FDE2B6CF}" name="Column4" dataDxfId="6">
+    <tableColumn id="3" xr3:uid="{288D3A6C-7636-4CB2-9C87-1538FDE2B6CF}" name="Column4" dataDxfId="2">
       <calculatedColumnFormula>_xlfn.TEXTJOIN(,TRUE,$A14,E14,$H14)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{CDAAB1AB-3350-49D3-9504-F6B12A67CFE7}" name="Column5" dataDxfId="1">
       <calculatedColumnFormula>_xlfn.TEXTJOIN(,TRUE,$A14,F14,$H14)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{F016F048-ABEE-4E9F-8006-40199839670A}" name="Column6" dataDxfId="5">
+    <tableColumn id="5" xr3:uid="{F016F048-ABEE-4E9F-8006-40199839670A}" name="Column6" dataDxfId="0">
       <calculatedColumnFormula>_xlfn.CONCAT($A14,G14*100,$H14)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -808,7 +806,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -826,53 +824,53 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="I1" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="I2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" t="s">
-        <v>11</v>
-      </c>
       <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
         <v>14</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>15</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>16</v>
-      </c>
-      <c r="N2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I3" t="str">
         <f>B3</f>
@@ -901,223 +899,223 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>50000</v>
       </c>
       <c r="D4">
-        <v>3.7199999999999997E-2</v>
+        <v>1.4500000000000001E-2</v>
       </c>
       <c r="E4">
-        <v>9.64E-2</v>
+        <v>9.6500000000000002E-2</v>
       </c>
       <c r="F4">
         <f>E4-D4</f>
-        <v>5.9200000000000003E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="G4" s="3">
         <f>ROUND(F4/E4,3)</f>
-        <v>0.61399999999999999</v>
+        <v>0.85</v>
       </c>
       <c r="H4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I4" t="s">
         <v>0</v>
       </c>
       <c r="J4" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A4,C4,$H4)</f>
+        <f t="shared" ref="J4:J10" si="1">_xlfn.TEXTJOIN(,TRUE,$A4,C4,$H4)</f>
         <v>\num{50000}</v>
       </c>
       <c r="K4" t="str">
         <f>_xlfn.TEXTJOIN(,TRUE,$A4,D4,$H4)</f>
-        <v>\num{0.0372}</v>
+        <v>\num{0.0145}</v>
       </c>
       <c r="L4" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A4,E4,$H4)</f>
-        <v>\num{0.0964}</v>
+        <f t="shared" ref="L4:M7" si="2">_xlfn.TEXTJOIN(,TRUE,$A4,E4,$H4)</f>
+        <v>\num{0.0965}</v>
       </c>
       <c r="M4" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A4,F4,$H4)</f>
-        <v>\num{0.0592}</v>
+        <f t="shared" si="2"/>
+        <v>\num{0.082}</v>
       </c>
       <c r="N4" t="str">
         <f>_xlfn.CONCAT($A4,G4*100,$H4)</f>
-        <v>\num{61.4}</v>
+        <v>\num{85}</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>50000</v>
       </c>
       <c r="D5">
-        <v>4.1799999999999997E-2</v>
+        <v>1.4500000000000001E-2</v>
       </c>
       <c r="E5">
-        <v>9.64E-2</v>
+        <v>9.6500000000000002E-2</v>
       </c>
       <c r="F5">
         <f>E5-D5</f>
-        <v>5.4600000000000003E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" ref="G5:G10" si="1">ROUND(F5/E5,3)</f>
-        <v>0.56599999999999995</v>
+        <f t="shared" ref="G5:G10" si="3">ROUND(F5/E5,3)</f>
+        <v>0.85</v>
       </c>
       <c r="H5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I5" t="s">
         <v>1</v>
       </c>
       <c r="J5" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A5,C5,$H5)</f>
+        <f t="shared" si="1"/>
         <v>\num{50000}</v>
       </c>
       <c r="K5" t="str">
         <f>_xlfn.TEXTJOIN(,TRUE,$A5,D5,$H5)</f>
-        <v>\num{0.0418}</v>
+        <v>\num{0.0145}</v>
       </c>
       <c r="L5" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A5,E5,$H5)</f>
-        <v>\num{0.0964}</v>
+        <f t="shared" si="2"/>
+        <v>\num{0.0965}</v>
       </c>
       <c r="M5" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A5,F5,$H5)</f>
-        <v>\num{0.0546}</v>
+        <f t="shared" si="2"/>
+        <v>\num{0.082}</v>
       </c>
       <c r="N5" t="str">
         <f>_xlfn.CONCAT($A5,G5*100,$H5)</f>
-        <v>\num{56.6}</v>
+        <v>\num{85}</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <v>50000</v>
       </c>
       <c r="D6">
-        <v>4.7E-2</v>
+        <v>2.23E-2</v>
       </c>
       <c r="E6">
-        <v>9.64E-2</v>
+        <v>9.6500000000000002E-2</v>
       </c>
       <c r="F6">
         <f>E6-D6</f>
-        <v>4.9399999999999999E-2</v>
+        <v>7.4200000000000002E-2</v>
       </c>
       <c r="G6" s="3">
-        <f t="shared" si="1"/>
-        <v>0.51200000000000001</v>
+        <f t="shared" si="3"/>
+        <v>0.76900000000000002</v>
       </c>
       <c r="H6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I6" t="s">
         <v>2</v>
       </c>
       <c r="J6" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A6,C6,$H6)</f>
+        <f t="shared" si="1"/>
         <v>\num{50000}</v>
       </c>
       <c r="K6" t="str">
         <f>_xlfn.TEXTJOIN(,TRUE,$A6,D6,$H6)</f>
-        <v>\num{0.047}</v>
+        <v>\num{0.0223}</v>
       </c>
       <c r="L6" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A6,E6,$H6)</f>
-        <v>\num{0.0964}</v>
+        <f t="shared" si="2"/>
+        <v>\num{0.0965}</v>
       </c>
       <c r="M6" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A6,F6,$H6)</f>
-        <v>\num{0.0494}</v>
+        <f t="shared" si="2"/>
+        <v>\num{0.0742}</v>
       </c>
       <c r="N6" t="str">
         <f>_xlfn.CONCAT($A6,G6*100,$H6)</f>
-        <v>\num{51.2}</v>
+        <v>\num{76.9}</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>50000</v>
       </c>
       <c r="D7">
-        <v>5.7299999999999997E-2</v>
+        <v>3.0700000000000002E-2</v>
       </c>
       <c r="E7">
-        <v>9.64E-2</v>
+        <v>9.6500000000000002E-2</v>
       </c>
       <c r="F7">
         <f>E7-D7</f>
-        <v>3.9100000000000003E-2</v>
+        <v>6.5799999999999997E-2</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" si="1"/>
-        <v>0.40600000000000003</v>
+        <f t="shared" si="3"/>
+        <v>0.68200000000000005</v>
       </c>
       <c r="H7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I7" t="s">
         <v>3</v>
       </c>
       <c r="J7" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A7,C7,$H7)</f>
+        <f t="shared" si="1"/>
         <v>\num{50000}</v>
       </c>
       <c r="K7" t="str">
         <f>_xlfn.TEXTJOIN(,TRUE,$A7,D7,$H7)</f>
-        <v>\num{0.0573}</v>
+        <v>\num{0.0307}</v>
       </c>
       <c r="L7" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A7,E7,$H7)</f>
-        <v>\num{0.0964}</v>
+        <f t="shared" si="2"/>
+        <v>\num{0.0965}</v>
       </c>
       <c r="M7" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A7,F7,$H7)</f>
-        <v>\num{0.0391}</v>
+        <f t="shared" si="2"/>
+        <v>\num{0.0658}</v>
       </c>
       <c r="N7" t="str">
         <f>_xlfn.CONCAT($A7,G7*100,$H7)</f>
-        <v>\num{40.6}</v>
+        <v>\num{68.2}</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8">
         <v>180000</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8">
         <v>4.6600000000000003E-2</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I8" t="s">
         <v>4</v>
       </c>
       <c r="J8" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A8,C8,$H8)</f>
+        <f t="shared" si="1"/>
         <v>\num{180000}</v>
       </c>
       <c r="K8" s="4" t="str">
@@ -1139,7 +1137,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9">
         <v>17176</v>
@@ -1155,17 +1153,17 @@
         <v>1.3100000000000001E-2</v>
       </c>
       <c r="G9" s="3">
+        <f t="shared" si="3"/>
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="H9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" t="str">
         <f t="shared" si="1"/>
-        <v>0.21199999999999999</v>
-      </c>
-      <c r="H9" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" t="s">
-        <v>5</v>
-      </c>
-      <c r="J9" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A9,C9,$H9)</f>
         <v>\num{17176}</v>
       </c>
       <c r="K9" t="str">
@@ -1187,7 +1185,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10">
         <v>388</v>
@@ -1203,17 +1201,17 @@
         <v>7.7499999999999999E-2</v>
       </c>
       <c r="G10" s="3">
+        <f t="shared" si="3"/>
+        <v>0.442</v>
+      </c>
+      <c r="H10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" t="str">
         <f t="shared" si="1"/>
-        <v>0.442</v>
-      </c>
-      <c r="H10" t="s">
-        <v>8</v>
-      </c>
-      <c r="I10" t="s">
-        <v>6</v>
-      </c>
-      <c r="J10" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A10,C10,$H10)</f>
         <v>\num{388}</v>
       </c>
       <c r="K10" t="str">
@@ -1235,274 +1233,274 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="I12" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="I13" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" t="s">
         <v>10</v>
       </c>
-      <c r="J13" t="s">
-        <v>11</v>
-      </c>
       <c r="K13" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" t="s">
         <v>14</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>15</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>16</v>
-      </c>
-      <c r="N13" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" t="s">
         <v>22</v>
       </c>
-      <c r="E14" t="s">
-        <v>23</v>
-      </c>
       <c r="F14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" t="s">
         <v>26</v>
       </c>
-      <c r="G14" t="s">
-        <v>27</v>
-      </c>
       <c r="H14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I14" t="str">
         <f>B14</f>
         <v>Method</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" ref="J14:J21" si="2">_xlfn.TEXTJOIN(,TRUE,A14,C14,H14)</f>
+        <f t="shared" ref="J14:J21" si="4">_xlfn.TEXTJOIN(,TRUE,A14,C14,H14)</f>
         <v>\thead{\# \glspl{gb}}</v>
       </c>
       <c r="K14" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A14,D14,$H14)</f>
+        <f t="shared" ref="K14:K19" si="5">_xlfn.TEXTJOIN(,TRUE,$A14,D14,$H14)</f>
         <v>\thead{\gls{rmse} \\ (\SI{}{\J\per\square\meter})}</v>
       </c>
       <c r="L14" t="str">
-        <f t="shared" ref="L14:N14" si="3">_xlfn.TEXTJOIN(,TRUE,$A14,E14,$H14)</f>
+        <f t="shared" ref="L14:N14" si="6">_xlfn.TEXTJOIN(,TRUE,$A14,E14,$H14)</f>
         <v>\thead{Cst, Avg \gls{rmse} \\ (\SI{}{\J\per\square\meter})}</v>
       </c>
       <c r="M14" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>\thead{\gls{rmse} $\downarrow$ \\ (\SI{}{\J\per\square\meter})}</v>
       </c>
       <c r="N14" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>\thead{\gls{rmse} $\downarrow$ \\ (\%)}</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15">
         <v>50000</v>
       </c>
-      <c r="D15">
-        <v>5.4100000000000002E-2</v>
+      <c r="D15" s="7">
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="E15">
-        <v>0.12959999999999999</v>
+        <v>0.13020000000000001</v>
       </c>
       <c r="F15">
         <f>E15-D15</f>
-        <v>7.5499999999999984E-2</v>
+        <v>0.10820000000000002</v>
       </c>
       <c r="G15" s="3">
         <f>ROUND(F15/E15,3)</f>
-        <v>0.58299999999999996</v>
+        <v>0.83099999999999996</v>
       </c>
       <c r="H15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>0</v>
       </c>
       <c r="J15" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>\num{50000}</v>
       </c>
       <c r="K15" s="1" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A15,D15,$H15)</f>
-        <v>\num{0.0541}</v>
+        <f t="shared" si="5"/>
+        <v>\num{0.022}</v>
       </c>
       <c r="L15" s="1" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A15,E15,$H15)</f>
-        <v>\num{0.1296}</v>
+        <f t="shared" ref="L15:M19" si="7">_xlfn.TEXTJOIN(,TRUE,$A15,E15,$H15)</f>
+        <v>\num{0.1302}</v>
       </c>
       <c r="M15" s="1" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A15,F15,$H15)</f>
-        <v>\num{0.0755}</v>
+        <f t="shared" si="7"/>
+        <v>\num{0.1082}</v>
       </c>
       <c r="N15" s="2" t="str">
         <f>_xlfn.CONCAT($A15,G15*100,$H15)</f>
-        <v>\num{58.3}</v>
+        <v>\num{83.1}</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16">
         <v>50000</v>
       </c>
       <c r="D16">
-        <v>6.0699999999999997E-2</v>
+        <v>2.4199999999999999E-2</v>
       </c>
       <c r="E16">
-        <v>0.12959999999999999</v>
+        <v>0.13020000000000001</v>
       </c>
       <c r="F16">
         <f>E16-D16</f>
-        <v>6.8899999999999989E-2</v>
+        <v>0.10600000000000001</v>
       </c>
       <c r="G16" s="3">
-        <f t="shared" ref="G16:G21" si="4">ROUND(F16/E16,3)</f>
-        <v>0.53200000000000003</v>
+        <f t="shared" ref="G16:G21" si="8">ROUND(F16/E16,3)</f>
+        <v>0.81399999999999995</v>
       </c>
       <c r="H16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>1</v>
       </c>
       <c r="J16" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>\num{50000}</v>
       </c>
       <c r="K16" s="1" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A16,D16,$H16)</f>
-        <v>\num{0.0607}</v>
+        <f t="shared" si="5"/>
+        <v>\num{0.0242}</v>
       </c>
       <c r="L16" s="1" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A16,E16,$H16)</f>
-        <v>\num{0.1296}</v>
+        <f t="shared" si="7"/>
+        <v>\num{0.1302}</v>
       </c>
       <c r="M16" s="1" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A16,F16,$H16)</f>
-        <v>\num{0.0689}</v>
+        <f t="shared" si="7"/>
+        <v>\num{0.106}</v>
       </c>
       <c r="N16" s="2" t="str">
         <f>_xlfn.CONCAT($A16,G16*100,$H16)</f>
-        <v>\num{53.2}</v>
+        <v>\num{81.4}</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17">
         <v>50000</v>
       </c>
       <c r="D17">
-        <v>6.8000000000000005E-2</v>
+        <v>3.4500000000000003E-2</v>
       </c>
       <c r="E17">
-        <v>0.12959999999999999</v>
+        <v>0.13020000000000001</v>
       </c>
       <c r="F17">
         <f>E17-D17</f>
-        <v>6.1599999999999988E-2</v>
+        <v>9.5700000000000007E-2</v>
       </c>
       <c r="G17" s="3">
-        <f t="shared" si="4"/>
-        <v>0.47499999999999998</v>
+        <f t="shared" si="8"/>
+        <v>0.73499999999999999</v>
       </c>
       <c r="H17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>2</v>
       </c>
       <c r="J17" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>\num{50000}</v>
       </c>
       <c r="K17" s="1" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A17,D17,$H17)</f>
-        <v>\num{0.068}</v>
+        <f t="shared" si="5"/>
+        <v>\num{0.0345}</v>
       </c>
       <c r="L17" s="1" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A17,E17,$H17)</f>
-        <v>\num{0.1296}</v>
+        <f t="shared" si="7"/>
+        <v>\num{0.1302}</v>
       </c>
       <c r="M17" s="1" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A17,F17,$H17)</f>
-        <v>\num{0.0616}</v>
+        <f t="shared" si="7"/>
+        <v>\num{0.0957}</v>
       </c>
       <c r="N17" s="2" t="str">
         <f>_xlfn.CONCAT($A17,G17*100,$H17)</f>
-        <v>\num{47.5}</v>
+        <v>\num{73.5}</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18">
         <v>50000</v>
       </c>
       <c r="D18">
-        <v>8.2100000000000006E-2</v>
+        <v>4.48E-2</v>
       </c>
       <c r="E18">
-        <v>0.12959999999999999</v>
+        <v>0.13020000000000001</v>
       </c>
       <c r="F18">
         <f>E18-D18</f>
-        <v>4.7499999999999987E-2</v>
+        <v>8.5400000000000004E-2</v>
       </c>
       <c r="G18" s="3">
-        <f t="shared" si="4"/>
-        <v>0.36699999999999999</v>
+        <f t="shared" si="8"/>
+        <v>0.65600000000000003</v>
       </c>
       <c r="H18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>3</v>
       </c>
       <c r="J18" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>\num{50000}</v>
       </c>
       <c r="K18" s="1" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A18,D18,$H18)</f>
-        <v>\num{0.0821}</v>
+        <f t="shared" si="5"/>
+        <v>\num{0.0448}</v>
       </c>
       <c r="L18" s="1" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A18,E18,$H18)</f>
-        <v>\num{0.1296}</v>
+        <f t="shared" si="7"/>
+        <v>\num{0.1302}</v>
       </c>
       <c r="M18" s="1" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A18,F18,$H18)</f>
-        <v>\num{0.0475}</v>
+        <f t="shared" si="7"/>
+        <v>\num{0.0854}</v>
       </c>
       <c r="N18" s="2" t="str">
         <f>_xlfn.CONCAT($A18,G18*100,$H18)</f>
-        <v>\num{36.7}</v>
+        <v>\num{65.6}</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19">
         <v>180000</v>
@@ -1518,29 +1516,29 @@
         <v>8.8400000000000006E-2</v>
       </c>
       <c r="G19" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>0.90600000000000003</v>
       </c>
       <c r="H19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>4</v>
       </c>
       <c r="J19" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>\num{180000}</v>
       </c>
       <c r="K19" s="1" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A19,D19,$H19)</f>
+        <f t="shared" si="5"/>
         <v>\num{0.0092}</v>
       </c>
       <c r="L19" s="1" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A19,E19,$H19)</f>
+        <f t="shared" si="7"/>
         <v>\num{0.0976}</v>
       </c>
       <c r="M19" s="1" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A19,F19,$H19)</f>
+        <f t="shared" si="7"/>
         <v>\num{0.0884}</v>
       </c>
       <c r="N19" s="2" t="str">
@@ -1550,31 +1548,31 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20">
         <v>17176</v>
       </c>
       <c r="D20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E20">
         <v>8.5400000000000004E-2</v>
       </c>
       <c r="F20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" t="s">
+        <v>7</v>
+      </c>
+      <c r="I20" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G20" t="s">
-        <v>28</v>
-      </c>
-      <c r="H20" t="s">
-        <v>8</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>5</v>
-      </c>
       <c r="J20" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>\num{17176}</v>
       </c>
       <c r="K20" s="1" t="str">
@@ -1596,7 +1594,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21">
         <v>388</v>
@@ -1612,17 +1610,17 @@
         <v>0.12659999999999999</v>
       </c>
       <c r="G21" s="3">
+        <f t="shared" si="8"/>
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="H21" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J21" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>0.56399999999999995</v>
-      </c>
-      <c r="H21" t="s">
-        <v>8</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="J21" s="1" t="str">
-        <f t="shared" si="2"/>
         <v>\num{388}</v>
       </c>
       <c r="K21" s="1" t="str">

</xml_diff>

<commit_message>
kim interp, metastability, degeneracy, dist ensemble
</commit_message>
<xml_diff>
--- a/error-compare.xlsx
+++ b/error-compare.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sterg\Documents\GitHub\infer\code\interp\code\interp5DOF-paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC673420-D59A-4C69-A345-41DCA8579356}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA614A1-B324-43E7-9247-89F642AF3BC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3FFA48DE-A732-4E48-AC34-6AA140314E0A}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <author>Sterling Baird</author>
   </authors>
   <commentList>
-    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{515906A6-986C-44A3-895C-93538E2AECCD}">
+    <comment ref="D24" authorId="0" shapeId="0" xr:uid="{515906A6-986C-44A3-895C-93538E2AECCD}">
       <text>
         <r>
           <rPr>
@@ -165,7 +165,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -247,7 +247,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,8 +457,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E2162E0-C385-4FAC-ABAF-ABB1A9A63773}" name="Table1" displayName="Table1" ref="I2:N10" totalsRowShown="0">
-  <autoFilter ref="I2:N10" xr:uid="{34723225-B821-40D5-8CA0-E779B3D75340}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0E2162E0-C385-4FAC-ABAF-ABB1A9A63773}" name="Table1" displayName="Table1" ref="I2:N9" totalsRowShown="0">
+  <autoFilter ref="I2:N9" xr:uid="{34723225-B821-40D5-8CA0-E779B3D75340}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{CE715634-CEAE-4F5C-BE92-319D9E9C6D95}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{857359D7-9BF3-4628-AEC1-B8C24263A700}" name="Column2">
@@ -482,24 +482,24 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{50286348-A0AD-4367-867A-FF703B492F79}" name="Table2" displayName="Table2" ref="I13:N21" totalsRowShown="0" dataDxfId="6">
-  <autoFilter ref="I13:N21" xr:uid="{62E6D853-2620-453D-94A0-2A9CC9A67D6A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{50286348-A0AD-4367-867A-FF703B492F79}" name="Table2" displayName="Table2" ref="I12:N19" totalsRowShown="0" dataDxfId="6">
+  <autoFilter ref="I12:N19" xr:uid="{62E6D853-2620-453D-94A0-2A9CC9A67D6A}"/>
   <tableColumns count="6">
     <tableColumn id="6" xr3:uid="{A9D0C93B-0EA4-4493-91CC-FEFD3AE97CC7}" name="Column1" dataDxfId="5"/>
     <tableColumn id="1" xr3:uid="{3314CF19-98B3-4633-8C5D-306394963DCF}" name="Column2" dataDxfId="4">
-      <calculatedColumnFormula>_xlfn.TEXTJOIN(,TRUE,A14,C14,H14)</calculatedColumnFormula>
+      <calculatedColumnFormula>_xlfn.TEXTJOIN(,TRUE,A13,C13,H13)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{62BC181E-E540-457E-8A83-80B02351069D}" name="Column3" dataDxfId="3">
-      <calculatedColumnFormula>_xlfn.TEXTJOIN(,TRUE,$A14,D14,$H14)</calculatedColumnFormula>
+      <calculatedColumnFormula>_xlfn.TEXTJOIN(,TRUE,$A13,D13,$H13)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{288D3A6C-7636-4CB2-9C87-1538FDE2B6CF}" name="Column4" dataDxfId="2">
-      <calculatedColumnFormula>_xlfn.TEXTJOIN(,TRUE,$A14,E14,$H14)</calculatedColumnFormula>
+      <calculatedColumnFormula>_xlfn.TEXTJOIN(,TRUE,$A13,E13,$H13)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{CDAAB1AB-3350-49D3-9504-F6B12A67CFE7}" name="Column5" dataDxfId="1">
-      <calculatedColumnFormula>_xlfn.TEXTJOIN(,TRUE,$A14,F14,$H14)</calculatedColumnFormula>
+      <calculatedColumnFormula>_xlfn.TEXTJOIN(,TRUE,$A13,F13,$H13)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{F016F048-ABEE-4E9F-8006-40199839670A}" name="Column6" dataDxfId="0">
-      <calculatedColumnFormula>_xlfn.CONCAT($A14,G14*100,$H14)</calculatedColumnFormula>
+      <calculatedColumnFormula>_xlfn.CONCAT($A13,G13*100,$H13)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -803,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA484C6-BA9C-46C6-A4A6-2565F599DD0D}">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -925,7 +925,7 @@
         <v>0</v>
       </c>
       <c r="J4" t="str">
-        <f t="shared" ref="J4:J10" si="1">_xlfn.TEXTJOIN(,TRUE,$A4,C4,$H4)</f>
+        <f t="shared" ref="J4:J9" si="1">_xlfn.TEXTJOIN(,TRUE,$A4,C4,$H4)</f>
         <v>\num{50000}</v>
       </c>
       <c r="K4" t="str">
@@ -963,7 +963,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" ref="G5:G10" si="3">ROUND(F5/E5,3)</f>
+        <f t="shared" ref="G5:G9" si="3">ROUND(F5/E5,3)</f>
         <v>0.85</v>
       </c>
       <c r="H5" t="s">
@@ -1094,45 +1094,47 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>180000</v>
-      </c>
-      <c r="D8" t="s">
-        <v>27</v>
+        <v>17176</v>
+      </c>
+      <c r="D8">
+        <v>4.8599999999999997E-2</v>
       </c>
       <c r="E8">
-        <v>4.6600000000000003E-2</v>
-      </c>
-      <c r="F8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" t="s">
-        <v>27</v>
+        <v>6.1699999999999998E-2</v>
+      </c>
+      <c r="F8">
+        <f>E8-D8</f>
+        <v>1.3100000000000001E-2</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="3"/>
+        <v>0.21199999999999999</v>
       </c>
       <c r="H8" t="s">
         <v>7</v>
       </c>
       <c r="I8" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="1"/>
-        <v>\num{180000}</v>
-      </c>
-      <c r="K8" s="4" t="str">
-        <f>D8</f>
-        <v>\NA</v>
+        <v>\num{17176}</v>
+      </c>
+      <c r="K8" t="str">
+        <f>_xlfn.TEXTJOIN(,TRUE,$A8,D8,$H8)</f>
+        <v>\num{0.0486}</v>
       </c>
       <c r="L8" t="str">
         <f>_xlfn.TEXTJOIN(,TRUE,$A8,E8,$H8)</f>
-        <v>\num{0.0466}</v>
-      </c>
-      <c r="M8" s="4" t="str">
-        <f>F8</f>
-        <v>\NA</v>
-      </c>
-      <c r="N8" s="4" t="str">
-        <f>G8</f>
-        <v>\NA</v>
+        <v>\num{0.0617}</v>
+      </c>
+      <c r="M8" t="str">
+        <f>_xlfn.TEXTJOIN(,TRUE,$A8,F8,$H8)</f>
+        <v>\num{0.0131}</v>
+      </c>
+      <c r="N8" t="str">
+        <f>_xlfn.CONCAT($A8,G8*100,$H8)</f>
+        <v>\num{21.2}</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -1140,170 +1142,170 @@
         <v>6</v>
       </c>
       <c r="C9">
-        <v>17176</v>
+        <v>388</v>
       </c>
       <c r="D9">
-        <v>4.8599999999999997E-2</v>
+        <v>9.7699999999999995E-2</v>
       </c>
       <c r="E9">
-        <v>6.1699999999999998E-2</v>
+        <v>0.17519999999999999</v>
       </c>
       <c r="F9">
         <f>E9-D9</f>
-        <v>1.3100000000000001E-2</v>
+        <v>7.7499999999999999E-2</v>
       </c>
       <c r="G9" s="3">
         <f t="shared" si="3"/>
-        <v>0.21199999999999999</v>
+        <v>0.442</v>
       </c>
       <c r="H9" t="s">
         <v>7</v>
       </c>
       <c r="I9" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="1"/>
-        <v>\num{17176}</v>
+        <v>\num{388}</v>
       </c>
       <c r="K9" t="str">
         <f>_xlfn.TEXTJOIN(,TRUE,$A9,D9,$H9)</f>
-        <v>\num{0.0486}</v>
+        <v>\num{0.0977}</v>
       </c>
       <c r="L9" t="str">
         <f>_xlfn.TEXTJOIN(,TRUE,$A9,E9,$H9)</f>
-        <v>\num{0.0617}</v>
+        <v>\num{0.1752}</v>
       </c>
       <c r="M9" t="str">
         <f>_xlfn.TEXTJOIN(,TRUE,$A9,F9,$H9)</f>
-        <v>\num{0.0131}</v>
+        <v>\num{0.0775}</v>
       </c>
       <c r="N9" t="str">
         <f>_xlfn.CONCAT($A9,G9*100,$H9)</f>
-        <v>\num{21.2}</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10">
-        <v>388</v>
-      </c>
-      <c r="D10">
-        <v>9.7699999999999995E-2</v>
-      </c>
-      <c r="E10">
-        <v>0.17519999999999999</v>
-      </c>
-      <c r="F10">
-        <f>E10-D10</f>
-        <v>7.7499999999999999E-2</v>
-      </c>
-      <c r="G10" s="3">
-        <f t="shared" si="3"/>
-        <v>0.442</v>
-      </c>
-      <c r="H10" t="s">
+        <v>\num{44.2}</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I11" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="I12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" t="s">
+        <v>10</v>
+      </c>
+      <c r="K12" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12" t="s">
+        <v>15</v>
+      </c>
+      <c r="N12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" t="s">
         <v>7</v>
       </c>
-      <c r="I10" t="s">
-        <v>5</v>
-      </c>
-      <c r="J10" t="str">
-        <f t="shared" si="1"/>
-        <v>\num{388}</v>
-      </c>
-      <c r="K10" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A10,D10,$H10)</f>
-        <v>\num{0.0977}</v>
-      </c>
-      <c r="L10" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A10,E10,$H10)</f>
-        <v>\num{0.1752}</v>
-      </c>
-      <c r="M10" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A10,F10,$H10)</f>
-        <v>\num{0.0775}</v>
-      </c>
-      <c r="N10" t="str">
-        <f>_xlfn.CONCAT($A10,G10*100,$H10)</f>
-        <v>\num{44.2}</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="I12" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="I13" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" t="s">
-        <v>10</v>
-      </c>
-      <c r="K13" t="s">
-        <v>13</v>
-      </c>
-      <c r="L13" t="s">
-        <v>14</v>
-      </c>
-      <c r="M13" t="s">
-        <v>15</v>
-      </c>
-      <c r="N13" t="s">
-        <v>16</v>
+      <c r="I13" t="str">
+        <f>B13</f>
+        <v>Method</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" ref="J13:J19" si="4">_xlfn.TEXTJOIN(,TRUE,A13,C13,H13)</f>
+        <v>\thead{\# \glspl{gb}}</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" ref="K13:K17" si="5">_xlfn.TEXTJOIN(,TRUE,$A13,D13,$H13)</f>
+        <v>\thead{\gls{rmse} \\ (\SI{}{\J\per\square\meter})}</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" ref="L13:N13" si="6">_xlfn.TEXTJOIN(,TRUE,$A13,E13,$H13)</f>
+        <v>\thead{Cst, Avg \gls{rmse} \\ (\SI{}{\J\per\square\meter})}</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" si="6"/>
+        <v>\thead{\gls{rmse} $\downarrow$ \\ (\SI{}{\J\per\square\meter})}</v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" si="6"/>
+        <v>\thead{\gls{rmse} $\downarrow$ \\ (\%)}</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" t="s">
-        <v>26</v>
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>50000</v>
+      </c>
+      <c r="D14" s="7">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E14">
+        <v>0.13020000000000001</v>
+      </c>
+      <c r="F14">
+        <f>E14-D14</f>
+        <v>0.10820000000000002</v>
+      </c>
+      <c r="G14" s="3">
+        <f>ROUND(F14/E14,3)</f>
+        <v>0.83099999999999996</v>
       </c>
       <c r="H14" t="s">
         <v>7</v>
       </c>
-      <c r="I14" t="str">
-        <f>B14</f>
-        <v>Method</v>
-      </c>
-      <c r="J14" t="str">
-        <f t="shared" ref="J14:J21" si="4">_xlfn.TEXTJOIN(,TRUE,A14,C14,H14)</f>
-        <v>\thead{\# \glspl{gb}}</v>
-      </c>
-      <c r="K14" t="str">
-        <f t="shared" ref="K14:K19" si="5">_xlfn.TEXTJOIN(,TRUE,$A14,D14,$H14)</f>
-        <v>\thead{\gls{rmse} \\ (\SI{}{\J\per\square\meter})}</v>
-      </c>
-      <c r="L14" t="str">
-        <f t="shared" ref="L14:N14" si="6">_xlfn.TEXTJOIN(,TRUE,$A14,E14,$H14)</f>
-        <v>\thead{Cst, Avg \gls{rmse} \\ (\SI{}{\J\per\square\meter})}</v>
-      </c>
-      <c r="M14" t="str">
-        <f t="shared" si="6"/>
-        <v>\thead{\gls{rmse} $\downarrow$ \\ (\SI{}{\J\per\square\meter})}</v>
-      </c>
-      <c r="N14" t="str">
-        <f t="shared" si="6"/>
-        <v>\thead{\gls{rmse} $\downarrow$ \\ (\%)}</v>
+      <c r="I14" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v>\num{50000}</v>
+      </c>
+      <c r="K14" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v>\num{0.022}</v>
+      </c>
+      <c r="L14" s="1" t="str">
+        <f t="shared" ref="L14:M17" si="7">_xlfn.TEXTJOIN(,TRUE,$A14,E14,$H14)</f>
+        <v>\num{0.1302}</v>
+      </c>
+      <c r="M14" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>\num{0.1082}</v>
+      </c>
+      <c r="N14" s="2" t="str">
+        <f>_xlfn.CONCAT($A14,G14*100,$H14)</f>
+        <v>\num{83.1}</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -1313,25 +1315,25 @@
       <c r="C15">
         <v>50000</v>
       </c>
-      <c r="D15" s="7">
-        <v>2.1999999999999999E-2</v>
+      <c r="D15">
+        <v>2.4199999999999999E-2</v>
       </c>
       <c r="E15">
         <v>0.13020000000000001</v>
       </c>
       <c r="F15">
         <f>E15-D15</f>
-        <v>0.10820000000000002</v>
+        <v>0.10600000000000001</v>
       </c>
       <c r="G15" s="3">
-        <f>ROUND(F15/E15,3)</f>
-        <v>0.83099999999999996</v>
+        <f t="shared" ref="G15:G19" si="8">ROUND(F15/E15,3)</f>
+        <v>0.81399999999999995</v>
       </c>
       <c r="H15" t="s">
         <v>7</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" s="1" t="str">
         <f t="shared" si="4"/>
@@ -1339,19 +1341,19 @@
       </c>
       <c r="K15" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>\num{0.022}</v>
+        <v>\num{0.0242}</v>
       </c>
       <c r="L15" s="1" t="str">
-        <f t="shared" ref="L15:M19" si="7">_xlfn.TEXTJOIN(,TRUE,$A15,E15,$H15)</f>
+        <f t="shared" si="7"/>
         <v>\num{0.1302}</v>
       </c>
       <c r="M15" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>\num{0.1082}</v>
+        <v>\num{0.106}</v>
       </c>
       <c r="N15" s="2" t="str">
         <f>_xlfn.CONCAT($A15,G15*100,$H15)</f>
-        <v>\num{83.1}</v>
+        <v>\num{81.4}</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
@@ -1362,24 +1364,24 @@
         <v>50000</v>
       </c>
       <c r="D16">
-        <v>2.4199999999999999E-2</v>
+        <v>3.4500000000000003E-2</v>
       </c>
       <c r="E16">
         <v>0.13020000000000001</v>
       </c>
       <c r="F16">
         <f>E16-D16</f>
-        <v>0.10600000000000001</v>
+        <v>9.5700000000000007E-2</v>
       </c>
       <c r="G16" s="3">
-        <f t="shared" ref="G16:G21" si="8">ROUND(F16/E16,3)</f>
-        <v>0.81399999999999995</v>
+        <f t="shared" si="8"/>
+        <v>0.73499999999999999</v>
       </c>
       <c r="H16" t="s">
         <v>7</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J16" s="1" t="str">
         <f t="shared" si="4"/>
@@ -1387,7 +1389,7 @@
       </c>
       <c r="K16" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>\num{0.0242}</v>
+        <v>\num{0.0345}</v>
       </c>
       <c r="L16" s="1" t="str">
         <f t="shared" si="7"/>
@@ -1395,11 +1397,11 @@
       </c>
       <c r="M16" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>\num{0.106}</v>
+        <v>\num{0.0957}</v>
       </c>
       <c r="N16" s="2" t="str">
         <f>_xlfn.CONCAT($A16,G16*100,$H16)</f>
-        <v>\num{81.4}</v>
+        <v>\num{73.5}</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
@@ -1410,24 +1412,24 @@
         <v>50000</v>
       </c>
       <c r="D17">
-        <v>3.4500000000000003E-2</v>
+        <v>4.48E-2</v>
       </c>
       <c r="E17">
         <v>0.13020000000000001</v>
       </c>
       <c r="F17">
         <f>E17-D17</f>
-        <v>9.5700000000000007E-2</v>
+        <v>8.5400000000000004E-2</v>
       </c>
       <c r="G17" s="3">
         <f t="shared" si="8"/>
-        <v>0.73499999999999999</v>
+        <v>0.65600000000000003</v>
       </c>
       <c r="H17" t="s">
         <v>7</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J17" s="1" t="str">
         <f t="shared" si="4"/>
@@ -1435,7 +1437,7 @@
       </c>
       <c r="K17" s="1" t="str">
         <f t="shared" si="5"/>
-        <v>\num{0.0345}</v>
+        <v>\num{0.0448}</v>
       </c>
       <c r="L17" s="1" t="str">
         <f t="shared" si="7"/>
@@ -1443,11 +1445,11 @@
       </c>
       <c r="M17" s="1" t="str">
         <f t="shared" si="7"/>
-        <v>\num{0.0957}</v>
+        <v>\num{0.0854}</v>
       </c>
       <c r="N17" s="2" t="str">
         <f>_xlfn.CONCAT($A17,G17*100,$H17)</f>
-        <v>\num{73.5}</v>
+        <v>\num{65.6}</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
@@ -1455,47 +1457,45 @@
         <v>6</v>
       </c>
       <c r="C18">
-        <v>50000</v>
-      </c>
-      <c r="D18">
-        <v>4.48E-2</v>
+        <v>17176</v>
+      </c>
+      <c r="D18" t="s">
+        <v>27</v>
       </c>
       <c r="E18">
-        <v>0.13020000000000001</v>
-      </c>
-      <c r="F18">
-        <f>E18-D18</f>
         <v>8.5400000000000004E-2</v>
       </c>
-      <c r="G18" s="3">
-        <f t="shared" si="8"/>
-        <v>0.65600000000000003</v>
+      <c r="F18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" t="s">
+        <v>27</v>
       </c>
       <c r="H18" t="s">
         <v>7</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="J18" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>\num{50000}</v>
+        <v>\num{17176}</v>
       </c>
       <c r="K18" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>\num{0.0448}</v>
+        <f>D18</f>
+        <v>\NA</v>
       </c>
       <c r="L18" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>\num{0.1302}</v>
-      </c>
-      <c r="M18" s="1" t="str">
-        <f t="shared" si="7"/>
+        <f>_xlfn.TEXTJOIN(,TRUE,$A18,E18,$H18)</f>
         <v>\num{0.0854}</v>
       </c>
-      <c r="N18" s="2" t="str">
-        <f>_xlfn.CONCAT($A18,G18*100,$H18)</f>
-        <v>\num{65.6}</v>
+      <c r="M18" s="4" t="str">
+        <f>F18</f>
+        <v>\NA</v>
+      </c>
+      <c r="N18" s="4" t="str">
+        <f>G18</f>
+        <v>\NA</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
@@ -1503,141 +1503,141 @@
         <v>6</v>
       </c>
       <c r="C19">
-        <v>180000</v>
+        <v>388</v>
       </c>
       <c r="D19">
-        <v>9.1999999999999998E-3</v>
+        <v>9.7699999999999995E-2</v>
       </c>
       <c r="E19">
-        <v>9.7600000000000006E-2</v>
+        <v>0.2243</v>
       </c>
       <c r="F19">
         <f>E19-D19</f>
-        <v>8.8400000000000006E-2</v>
+        <v>0.12659999999999999</v>
       </c>
       <c r="G19" s="3">
         <f t="shared" si="8"/>
-        <v>0.90600000000000003</v>
+        <v>0.56399999999999995</v>
       </c>
       <c r="H19" t="s">
         <v>7</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J19" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>\num{180000}</v>
+        <v>\num{388}</v>
       </c>
       <c r="K19" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>\num{0.0092}</v>
+        <f>_xlfn.TEXTJOIN(,TRUE,$A19,D19,$H19)</f>
+        <v>\num{0.0977}</v>
       </c>
       <c r="L19" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>\num{0.0976}</v>
+        <f>_xlfn.TEXTJOIN(,TRUE,$A19,E19,$H19)</f>
+        <v>\num{0.2243}</v>
       </c>
       <c r="M19" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>\num{0.0884}</v>
+        <f>_xlfn.TEXTJOIN(,TRUE,$A19,F19,$H19)</f>
+        <v>\num{0.1266}</v>
       </c>
       <c r="N19" s="2" t="str">
         <f>_xlfn.CONCAT($A19,G19*100,$H19)</f>
+        <v>\num{56.4}</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22">
+        <v>180000</v>
+      </c>
+      <c r="D22" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22">
+        <v>4.6600000000000003E-2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" t="s">
+        <v>7</v>
+      </c>
+      <c r="I22" t="s">
+        <v>4</v>
+      </c>
+      <c r="J22" t="str">
+        <f>_xlfn.TEXTJOIN(,TRUE,$A22,C22,$H22)</f>
+        <v>\num{180000}</v>
+      </c>
+      <c r="K22" s="4" t="str">
+        <f>D22</f>
+        <v>\NA</v>
+      </c>
+      <c r="L22" t="str">
+        <f>_xlfn.TEXTJOIN(,TRUE,$A22,E22,$H22)</f>
+        <v>\num{0.0466}</v>
+      </c>
+      <c r="M22" s="4" t="str">
+        <f>F22</f>
+        <v>\NA</v>
+      </c>
+      <c r="N22" s="4" t="str">
+        <f>G22</f>
+        <v>\NA</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24">
+        <v>180000</v>
+      </c>
+      <c r="D24">
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="E24">
+        <v>9.7600000000000006E-2</v>
+      </c>
+      <c r="F24">
+        <f>E24-D24</f>
+        <v>8.8400000000000006E-2</v>
+      </c>
+      <c r="G24" s="3">
+        <f>ROUND(F24/E24,3)</f>
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="H24" t="s">
+        <v>7</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J24" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(,TRUE,A24,C24,H24)</f>
+        <v>\num{180000}</v>
+      </c>
+      <c r="K24" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(,TRUE,$A24,D24,$H24)</f>
+        <v>\num{0.0092}</v>
+      </c>
+      <c r="L24" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(,TRUE,$A24,E24,$H24)</f>
+        <v>\num{0.0976}</v>
+      </c>
+      <c r="M24" s="1" t="str">
+        <f>_xlfn.TEXTJOIN(,TRUE,$A24,F24,$H24)</f>
+        <v>\num{0.0884}</v>
+      </c>
+      <c r="N24" s="2" t="str">
+        <f>_xlfn.CONCAT($A24,G24*100,$H24)</f>
         <v>\num{90.6}</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20">
-        <v>17176</v>
-      </c>
-      <c r="D20" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20">
-        <v>8.5400000000000004E-2</v>
-      </c>
-      <c r="F20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G20" t="s">
-        <v>27</v>
-      </c>
-      <c r="H20" t="s">
-        <v>7</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J20" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>\num{17176}</v>
-      </c>
-      <c r="K20" s="1" t="str">
-        <f>D20</f>
-        <v>\NA</v>
-      </c>
-      <c r="L20" s="1" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A20,E20,$H20)</f>
-        <v>\num{0.0854}</v>
-      </c>
-      <c r="M20" s="4" t="str">
-        <f>F20</f>
-        <v>\NA</v>
-      </c>
-      <c r="N20" s="4" t="str">
-        <f>G20</f>
-        <v>\NA</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21">
-        <v>388</v>
-      </c>
-      <c r="D21">
-        <v>9.7699999999999995E-2</v>
-      </c>
-      <c r="E21">
-        <v>0.2243</v>
-      </c>
-      <c r="F21">
-        <f>E21-D21</f>
-        <v>0.12659999999999999</v>
-      </c>
-      <c r="G21" s="3">
-        <f t="shared" si="8"/>
-        <v>0.56399999999999995</v>
-      </c>
-      <c r="H21" t="s">
-        <v>7</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J21" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>\num{388}</v>
-      </c>
-      <c r="K21" s="1" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A21,D21,$H21)</f>
-        <v>\num{0.0977}</v>
-      </c>
-      <c r="L21" s="1" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A21,E21,$H21)</f>
-        <v>\num{0.2243}</v>
-      </c>
-      <c r="M21" s="1" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A21,F21,$H21)</f>
-        <v>\num{0.1266}</v>
-      </c>
-      <c r="N21" s="2" t="str">
-        <f>_xlfn.CONCAT($A21,G21*100,$H21)</f>
-        <v>\num{56.4}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update tables and fix figure label issue
</commit_message>
<xml_diff>
--- a/error-compare.xlsx
+++ b/error-compare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sterg\Documents\GitHub\infer\code\interp\code\interp5DOF-paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA614A1-B324-43E7-9247-89F642AF3BC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91634C44-ADB1-4113-8307-4E6A197A1203}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3FFA48DE-A732-4E48-AC34-6AA140314E0A}"/>
   </bookViews>
@@ -805,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA484C6-BA9C-46C6-A4A6-2565F599DD0D}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -881,19 +881,19 @@
         <v>\# \glspl{gb}</v>
       </c>
       <c r="K3" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A3,D3,$H3)</f>
+        <f t="shared" ref="K3:K9" si="0">_xlfn.TEXTJOIN(,TRUE,$A3,D3,$H3)</f>
         <v>\thead{\gls{mae} \\ (\SI{}{\J\per\square\meter})}</v>
       </c>
       <c r="L3" t="str">
-        <f t="shared" ref="L3:N3" si="0">_xlfn.TEXTJOIN(,TRUE,$A3,E3,$H3)</f>
+        <f t="shared" ref="L3:N3" si="1">_xlfn.TEXTJOIN(,TRUE,$A3,E3,$H3)</f>
         <v>\thead{Cst, Avg \gls{mae} \\ (\SI{}{\J\per\square\meter})}</v>
       </c>
       <c r="M3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>\thead{\gls{mae} $\downarrow$ \\ (\SI{}{\J\per\square\meter})}</v>
       </c>
       <c r="N3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>\thead{\gls{mae} $\downarrow$ \\ (\%)}</v>
       </c>
     </row>
@@ -908,15 +908,15 @@
         <v>1.4500000000000001E-2</v>
       </c>
       <c r="E4">
-        <v>9.6500000000000002E-2</v>
+        <v>9.5500000000000002E-2</v>
       </c>
       <c r="F4">
-        <f>E4-D4</f>
-        <v>8.2000000000000003E-2</v>
+        <f t="shared" ref="F4:F9" si="2">E4-D4</f>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="G4" s="3">
         <f>ROUND(F4/E4,3)</f>
-        <v>0.85</v>
+        <v>0.84799999999999998</v>
       </c>
       <c r="H4" t="s">
         <v>7</v>
@@ -925,24 +925,24 @@
         <v>0</v>
       </c>
       <c r="J4" t="str">
-        <f t="shared" ref="J4:J9" si="1">_xlfn.TEXTJOIN(,TRUE,$A4,C4,$H4)</f>
+        <f t="shared" ref="J4:J9" si="3">_xlfn.TEXTJOIN(,TRUE,$A4,C4,$H4)</f>
         <v>\num{50000}</v>
       </c>
       <c r="K4" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A4,D4,$H4)</f>
+        <f t="shared" si="0"/>
         <v>\num{0.0145}</v>
       </c>
       <c r="L4" t="str">
-        <f t="shared" ref="L4:M7" si="2">_xlfn.TEXTJOIN(,TRUE,$A4,E4,$H4)</f>
-        <v>\num{0.0965}</v>
+        <f t="shared" ref="L4:M7" si="4">_xlfn.TEXTJOIN(,TRUE,$A4,E4,$H4)</f>
+        <v>\num{0.0955}</v>
       </c>
       <c r="M4" t="str">
-        <f t="shared" si="2"/>
-        <v>\num{0.082}</v>
+        <f t="shared" si="4"/>
+        <v>\num{0.081}</v>
       </c>
       <c r="N4" t="str">
-        <f>_xlfn.CONCAT($A4,G4*100,$H4)</f>
-        <v>\num{85}</v>
+        <f t="shared" ref="N4:N9" si="5">_xlfn.CONCAT($A4,G4*100,$H4)</f>
+        <v>\num{84.8}</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -956,15 +956,15 @@
         <v>1.4500000000000001E-2</v>
       </c>
       <c r="E5">
-        <v>9.6500000000000002E-2</v>
+        <v>9.5500000000000002E-2</v>
       </c>
       <c r="F5">
-        <f>E5-D5</f>
-        <v>8.2000000000000003E-2</v>
+        <f t="shared" si="2"/>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="G5" s="3">
-        <f t="shared" ref="G5:G9" si="3">ROUND(F5/E5,3)</f>
-        <v>0.85</v>
+        <f t="shared" ref="G5:G9" si="6">ROUND(F5/E5,3)</f>
+        <v>0.84799999999999998</v>
       </c>
       <c r="H5" t="s">
         <v>7</v>
@@ -973,24 +973,24 @@
         <v>1</v>
       </c>
       <c r="J5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>\num{50000}</v>
       </c>
       <c r="K5" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A5,D5,$H5)</f>
+        <f t="shared" si="0"/>
         <v>\num{0.0145}</v>
       </c>
       <c r="L5" t="str">
-        <f t="shared" si="2"/>
-        <v>\num{0.0965}</v>
+        <f t="shared" si="4"/>
+        <v>\num{0.0955}</v>
       </c>
       <c r="M5" t="str">
-        <f t="shared" si="2"/>
-        <v>\num{0.082}</v>
+        <f t="shared" si="4"/>
+        <v>\num{0.081}</v>
       </c>
       <c r="N5" t="str">
-        <f>_xlfn.CONCAT($A5,G5*100,$H5)</f>
-        <v>\num{85}</v>
+        <f t="shared" si="5"/>
+        <v>\num{84.8}</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
@@ -1001,18 +1001,18 @@
         <v>50000</v>
       </c>
       <c r="D6">
-        <v>2.23E-2</v>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="E6">
-        <v>9.6500000000000002E-2</v>
+        <v>9.5500000000000002E-2</v>
       </c>
       <c r="F6">
-        <f>E6-D6</f>
-        <v>7.4200000000000002E-2</v>
+        <f t="shared" si="2"/>
+        <v>7.3000000000000009E-2</v>
       </c>
       <c r="G6" s="3">
-        <f t="shared" si="3"/>
-        <v>0.76900000000000002</v>
+        <f t="shared" si="6"/>
+        <v>0.76400000000000001</v>
       </c>
       <c r="H6" t="s">
         <v>7</v>
@@ -1021,24 +1021,24 @@
         <v>2</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>\num{50000}</v>
       </c>
       <c r="K6" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A6,D6,$H6)</f>
-        <v>\num{0.0223}</v>
+        <f t="shared" si="0"/>
+        <v>\num{0.0225}</v>
       </c>
       <c r="L6" t="str">
-        <f t="shared" si="2"/>
-        <v>\num{0.0965}</v>
+        <f t="shared" si="4"/>
+        <v>\num{0.0955}</v>
       </c>
       <c r="M6" t="str">
-        <f t="shared" si="2"/>
-        <v>\num{0.0742}</v>
+        <f t="shared" si="4"/>
+        <v>\num{0.073}</v>
       </c>
       <c r="N6" t="str">
-        <f>_xlfn.CONCAT($A6,G6*100,$H6)</f>
-        <v>\num{76.9}</v>
+        <f t="shared" si="5"/>
+        <v>\num{76.4}</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
@@ -1052,15 +1052,15 @@
         <v>3.0700000000000002E-2</v>
       </c>
       <c r="E7">
-        <v>9.6500000000000002E-2</v>
+        <v>9.5500000000000002E-2</v>
       </c>
       <c r="F7">
-        <f>E7-D7</f>
-        <v>6.5799999999999997E-2</v>
+        <f t="shared" si="2"/>
+        <v>6.4799999999999996E-2</v>
       </c>
       <c r="G7" s="3">
-        <f t="shared" si="3"/>
-        <v>0.68200000000000005</v>
+        <f t="shared" si="6"/>
+        <v>0.67900000000000005</v>
       </c>
       <c r="H7" t="s">
         <v>7</v>
@@ -1069,24 +1069,24 @@
         <v>3</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>\num{50000}</v>
       </c>
       <c r="K7" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A7,D7,$H7)</f>
+        <f t="shared" si="0"/>
         <v>\num{0.0307}</v>
       </c>
       <c r="L7" t="str">
-        <f t="shared" si="2"/>
-        <v>\num{0.0965}</v>
+        <f t="shared" si="4"/>
+        <v>\num{0.0955}</v>
       </c>
       <c r="M7" t="str">
-        <f t="shared" si="2"/>
-        <v>\num{0.0658}</v>
+        <f t="shared" si="4"/>
+        <v>\num{0.0648}</v>
       </c>
       <c r="N7" t="str">
-        <f>_xlfn.CONCAT($A7,G7*100,$H7)</f>
-        <v>\num{68.2}</v>
+        <f t="shared" si="5"/>
+        <v>\num{67.9}</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -1103,11 +1103,11 @@
         <v>6.1699999999999998E-2</v>
       </c>
       <c r="F8">
-        <f>E8-D8</f>
+        <f t="shared" si="2"/>
         <v>1.3100000000000001E-2</v>
       </c>
       <c r="G8" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.21199999999999999</v>
       </c>
       <c r="H8" t="s">
@@ -1117,11 +1117,11 @@
         <v>28</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>\num{17176}</v>
       </c>
       <c r="K8" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A8,D8,$H8)</f>
+        <f t="shared" si="0"/>
         <v>\num{0.0486}</v>
       </c>
       <c r="L8" t="str">
@@ -1133,7 +1133,7 @@
         <v>\num{0.0131}</v>
       </c>
       <c r="N8" t="str">
-        <f>_xlfn.CONCAT($A8,G8*100,$H8)</f>
+        <f t="shared" si="5"/>
         <v>\num{21.2}</v>
       </c>
     </row>
@@ -1151,11 +1151,11 @@
         <v>0.17519999999999999</v>
       </c>
       <c r="F9">
-        <f>E9-D9</f>
+        <f t="shared" si="2"/>
         <v>7.7499999999999999E-2</v>
       </c>
       <c r="G9" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>0.442</v>
       </c>
       <c r="H9" t="s">
@@ -1165,11 +1165,11 @@
         <v>5</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>\num{388}</v>
       </c>
       <c r="K9" t="str">
-        <f>_xlfn.TEXTJOIN(,TRUE,$A9,D9,$H9)</f>
+        <f t="shared" si="0"/>
         <v>\num{0.0977}</v>
       </c>
       <c r="L9" t="str">
@@ -1181,7 +1181,7 @@
         <v>\num{0.0775}</v>
       </c>
       <c r="N9" t="str">
-        <f>_xlfn.CONCAT($A9,G9*100,$H9)</f>
+        <f t="shared" si="5"/>
         <v>\num{44.2}</v>
       </c>
     </row>
@@ -1240,23 +1240,23 @@
         <v>Method</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" ref="J13:J19" si="4">_xlfn.TEXTJOIN(,TRUE,A13,C13,H13)</f>
+        <f t="shared" ref="J13:J19" si="7">_xlfn.TEXTJOIN(,TRUE,A13,C13,H13)</f>
         <v>\thead{\# \glspl{gb}}</v>
       </c>
       <c r="K13" t="str">
-        <f t="shared" ref="K13:K17" si="5">_xlfn.TEXTJOIN(,TRUE,$A13,D13,$H13)</f>
+        <f t="shared" ref="K13:K17" si="8">_xlfn.TEXTJOIN(,TRUE,$A13,D13,$H13)</f>
         <v>\thead{\gls{rmse} \\ (\SI{}{\J\per\square\meter})}</v>
       </c>
       <c r="L13" t="str">
-        <f t="shared" ref="L13:N13" si="6">_xlfn.TEXTJOIN(,TRUE,$A13,E13,$H13)</f>
+        <f t="shared" ref="L13:N13" si="9">_xlfn.TEXTJOIN(,TRUE,$A13,E13,$H13)</f>
         <v>\thead{Cst, Avg \gls{rmse} \\ (\SI{}{\J\per\square\meter})}</v>
       </c>
       <c r="M13" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>\thead{\gls{rmse} $\downarrow$ \\ (\SI{}{\J\per\square\meter})}</v>
       </c>
       <c r="N13" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>\thead{\gls{rmse} $\downarrow$ \\ (\%)}</v>
       </c>
     </row>
@@ -1268,18 +1268,18 @@
         <v>50000</v>
       </c>
       <c r="D14" s="7">
-        <v>2.1999999999999999E-2</v>
+        <v>2.18E-2</v>
       </c>
       <c r="E14">
-        <v>0.13020000000000001</v>
+        <v>0.1283</v>
       </c>
       <c r="F14">
         <f>E14-D14</f>
-        <v>0.10820000000000002</v>
+        <v>0.1065</v>
       </c>
       <c r="G14" s="3">
         <f>ROUND(F14/E14,3)</f>
-        <v>0.83099999999999996</v>
+        <v>0.83</v>
       </c>
       <c r="H14" t="s">
         <v>7</v>
@@ -1288,24 +1288,24 @@
         <v>0</v>
       </c>
       <c r="J14" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>\num{50000}</v>
       </c>
       <c r="K14" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>\num{0.022}</v>
+        <f t="shared" si="8"/>
+        <v>\num{0.0218}</v>
       </c>
       <c r="L14" s="1" t="str">
-        <f t="shared" ref="L14:M17" si="7">_xlfn.TEXTJOIN(,TRUE,$A14,E14,$H14)</f>
-        <v>\num{0.1302}</v>
+        <f t="shared" ref="L14:M17" si="10">_xlfn.TEXTJOIN(,TRUE,$A14,E14,$H14)</f>
+        <v>\num{0.1283}</v>
       </c>
       <c r="M14" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>\num{0.1082}</v>
+        <f t="shared" si="10"/>
+        <v>\num{0.1065}</v>
       </c>
       <c r="N14" s="2" t="str">
         <f>_xlfn.CONCAT($A14,G14*100,$H14)</f>
-        <v>\num{83.1}</v>
+        <v>\num{83}</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -1316,17 +1316,17 @@
         <v>50000</v>
       </c>
       <c r="D15">
-        <v>2.4199999999999999E-2</v>
+        <v>2.3800000000000002E-2</v>
       </c>
       <c r="E15">
-        <v>0.13020000000000001</v>
+        <v>0.1283</v>
       </c>
       <c r="F15">
         <f>E15-D15</f>
-        <v>0.10600000000000001</v>
+        <v>0.1045</v>
       </c>
       <c r="G15" s="3">
-        <f t="shared" ref="G15:G19" si="8">ROUND(F15/E15,3)</f>
+        <f t="shared" ref="G15:G19" si="11">ROUND(F15/E15,3)</f>
         <v>0.81399999999999995</v>
       </c>
       <c r="H15" t="s">
@@ -1336,20 +1336,20 @@
         <v>1</v>
       </c>
       <c r="J15" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>\num{50000}</v>
       </c>
       <c r="K15" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>\num{0.0242}</v>
+        <f t="shared" si="8"/>
+        <v>\num{0.0238}</v>
       </c>
       <c r="L15" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>\num{0.1302}</v>
+        <f t="shared" si="10"/>
+        <v>\num{0.1283}</v>
       </c>
       <c r="M15" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>\num{0.106}</v>
+        <f t="shared" si="10"/>
+        <v>\num{0.1045}</v>
       </c>
       <c r="N15" s="2" t="str">
         <f>_xlfn.CONCAT($A15,G15*100,$H15)</f>
@@ -1364,18 +1364,18 @@
         <v>50000</v>
       </c>
       <c r="D16">
-        <v>3.4500000000000003E-2</v>
+        <v>3.56E-2</v>
       </c>
       <c r="E16">
-        <v>0.13020000000000001</v>
+        <v>0.1283</v>
       </c>
       <c r="F16">
         <f>E16-D16</f>
-        <v>9.5700000000000007E-2</v>
+        <v>9.2700000000000005E-2</v>
       </c>
       <c r="G16" s="3">
-        <f t="shared" si="8"/>
-        <v>0.73499999999999999</v>
+        <f t="shared" si="11"/>
+        <v>0.72299999999999998</v>
       </c>
       <c r="H16" t="s">
         <v>7</v>
@@ -1384,24 +1384,24 @@
         <v>2</v>
       </c>
       <c r="J16" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>\num{50000}</v>
       </c>
       <c r="K16" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>\num{0.0345}</v>
+        <f t="shared" si="8"/>
+        <v>\num{0.0356}</v>
       </c>
       <c r="L16" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>\num{0.1302}</v>
+        <f t="shared" si="10"/>
+        <v>\num{0.1283}</v>
       </c>
       <c r="M16" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>\num{0.0957}</v>
+        <f t="shared" si="10"/>
+        <v>\num{0.0927}</v>
       </c>
       <c r="N16" s="2" t="str">
         <f>_xlfn.CONCAT($A16,G16*100,$H16)</f>
-        <v>\num{73.5}</v>
+        <v>\num{72.3}</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
@@ -1412,18 +1412,18 @@
         <v>50000</v>
       </c>
       <c r="D17">
-        <v>4.48E-2</v>
+        <v>4.4499999999999998E-2</v>
       </c>
       <c r="E17">
-        <v>0.13020000000000001</v>
+        <v>0.1283</v>
       </c>
       <c r="F17">
         <f>E17-D17</f>
-        <v>8.5400000000000004E-2</v>
+        <v>8.3799999999999999E-2</v>
       </c>
       <c r="G17" s="3">
-        <f t="shared" si="8"/>
-        <v>0.65600000000000003</v>
+        <f t="shared" si="11"/>
+        <v>0.65300000000000002</v>
       </c>
       <c r="H17" t="s">
         <v>7</v>
@@ -1432,24 +1432,24 @@
         <v>3</v>
       </c>
       <c r="J17" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>\num{50000}</v>
       </c>
       <c r="K17" s="1" t="str">
-        <f t="shared" si="5"/>
-        <v>\num{0.0448}</v>
+        <f t="shared" si="8"/>
+        <v>\num{0.0445}</v>
       </c>
       <c r="L17" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>\num{0.1302}</v>
+        <f t="shared" si="10"/>
+        <v>\num{0.1283}</v>
       </c>
       <c r="M17" s="1" t="str">
-        <f t="shared" si="7"/>
-        <v>\num{0.0854}</v>
+        <f t="shared" si="10"/>
+        <v>\num{0.0838}</v>
       </c>
       <c r="N17" s="2" t="str">
         <f>_xlfn.CONCAT($A17,G17*100,$H17)</f>
-        <v>\num{65.6}</v>
+        <v>\num{65.3}</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
@@ -1478,7 +1478,7 @@
         <v>28</v>
       </c>
       <c r="J18" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>\num{17176}</v>
       </c>
       <c r="K18" s="1" t="str">
@@ -1516,7 +1516,7 @@
         <v>0.12659999999999999</v>
       </c>
       <c r="G19" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0.56399999999999995</v>
       </c>
       <c r="H19" t="s">
@@ -1526,7 +1526,7 @@
         <v>5</v>
       </c>
       <c r="J19" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>\num{388}</v>
       </c>
       <c r="K19" s="1" t="str">

</xml_diff>